<commit_message>
Changement des pins pour V12 nb 2
</commit_message>
<xml_diff>
--- a/Branchements.xlsx
+++ b/Branchements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Aller</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Vers Sortie Transfo Principal</t>
+  </si>
+  <si>
+    <t>Vers Alim Secours Transfo 12V</t>
   </si>
 </sst>
 </file>
@@ -315,38 +318,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -356,13 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,10 +716,10 @@
       <c r="R3" s="7"/>
     </row>
     <row r="4" spans="3:18">
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -733,8 +736,8 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="3:18">
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -751,8 +754,8 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="3:18">
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -807,31 +810,31 @@
     <row r="9" spans="3:18">
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="9"/>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="9"/>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="24" t="s">
         <v>1</v>
       </c>
       <c r="P9" s="9"/>
@@ -840,39 +843,34 @@
     </row>
     <row r="10" spans="3:18" ht="21" customHeight="1">
       <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
+      <c r="F10" s="25"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
+      <c r="I10" s="25"/>
       <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
+      <c r="L10" s="25"/>
       <c r="N10" s="23"/>
-      <c r="O10" s="24"/>
+      <c r="O10" s="25"/>
     </row>
     <row r="11" spans="3:18" ht="80.25" customHeight="1">
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="H11" s="14" t="s">
+      <c r="F11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="K11" s="14" t="s">
+      <c r="I11" s="26"/>
+      <c r="K11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="N11" s="14" t="s">
+      <c r="L11" s="26"/>
+      <c r="N11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="14"/>
+      <c r="O11" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C4:D6"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="H11:I11"/>
@@ -881,6 +879,11 @@
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="O9:O10"/>
+    <mergeCell ref="C4:D6"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -892,7 +895,7 @@
   <dimension ref="B2:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AU10" sqref="AU10"/>
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -965,40 +968,40 @@
     </row>
     <row r="3" spans="2:45" ht="7.5" customHeight="1">
       <c r="B3" s="5"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="7"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="7"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="7"/>
       <c r="AC3" s="5"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="7"/>
       <c r="AL3" s="5"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="28"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
       <c r="AO3" s="6"/>
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
@@ -1049,64 +1052,64 @@
     </row>
     <row r="5" spans="2:45" ht="79.5" customHeight="1">
       <c r="B5" s="5"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="25" t="s">
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="7"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="26"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="25" t="s">
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
       <c r="R5" s="7"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="26"/>
-      <c r="W5" s="27"/>
-      <c r="X5" s="25" t="s">
+      <c r="V5" s="29"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="27"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="30"/>
       <c r="AA5" s="7"/>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="25" t="s">
+      <c r="AD5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="25" t="s">
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="27"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="30"/>
       <c r="AJ5" s="7"/>
       <c r="AL5" s="5"/>
-      <c r="AM5" s="25" t="s">
+      <c r="AM5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AN5" s="26"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="25" t="s">
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="30"/>
+      <c r="AP5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="27"/>
+      <c r="AQ5" s="29"/>
+      <c r="AR5" s="30"/>
       <c r="AS5" s="7"/>
     </row>
     <row r="6" spans="2:45" ht="4.5" customHeight="1">
@@ -1195,206 +1198,182 @@
     </row>
     <row r="8" spans="2:45" s="6" customFormat="1" ht="6" customHeight="1">
       <c r="B8" s="5"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="7"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
       <c r="R8" s="7"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
       <c r="AA8" s="7"/>
       <c r="AC8" s="5"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="30"/>
-      <c r="AG8" s="30"/>
-      <c r="AH8" s="30"/>
-      <c r="AI8" s="30"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="15"/>
       <c r="AJ8" s="7"/>
       <c r="AL8" s="5"/>
-      <c r="AM8" s="30"/>
-      <c r="AN8" s="30"/>
-      <c r="AO8" s="30"/>
-      <c r="AP8" s="30"/>
-      <c r="AQ8" s="30"/>
-      <c r="AR8" s="30"/>
+      <c r="AM8" s="15"/>
+      <c r="AN8" s="15"/>
+      <c r="AO8" s="15"/>
+      <c r="AP8" s="15"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
       <c r="AS8" s="7"/>
     </row>
     <row r="9" spans="2:45" s="6" customFormat="1" ht="7.5" customHeight="1">
       <c r="B9" s="8"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="10"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="29" t="s">
+      <c r="P9" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="29" t="s">
+      <c r="Q9" s="27" t="s">
         <v>18</v>
       </c>
       <c r="R9" s="10"/>
       <c r="T9" s="8"/>
-      <c r="U9" s="29" t="s">
+      <c r="U9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="V9" s="29" t="s">
+      <c r="V9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="W9" s="29" t="s">
+      <c r="W9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="X9" s="29" t="s">
+      <c r="X9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="Y9" s="29" t="s">
+      <c r="Y9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="Z9" s="29" t="s">
+      <c r="Z9" s="27" t="s">
         <v>24</v>
       </c>
       <c r="AA9" s="10"/>
       <c r="AC9" s="8"/>
-      <c r="AD9" s="29" t="s">
+      <c r="AD9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="AE9" s="29" t="s">
+      <c r="AE9" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AF9" s="29" t="s">
+      <c r="AF9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AG9" s="29" t="s">
+      <c r="AG9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AH9" s="29" t="s">
+      <c r="AH9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AI9" s="29" t="s">
+      <c r="AI9" s="27" t="s">
         <v>26</v>
       </c>
       <c r="AJ9" s="10"/>
       <c r="AL9" s="8"/>
-      <c r="AM9" s="29" t="s">
+      <c r="AM9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="AN9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO9" s="29" t="s">
+      <c r="AN9" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AP9" s="29" t="s">
+      <c r="AP9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AQ9" s="29" t="s">
+      <c r="AQ9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="AR9" s="29" t="s">
+      <c r="AR9" s="27" t="s">
         <v>31</v>
       </c>
       <c r="AS9" s="10"/>
     </row>
     <row r="10" spans="2:45" ht="144.75" customHeight="1">
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AD10" s="29"/>
-      <c r="AE10" s="29"/>
-      <c r="AF10" s="29"/>
-      <c r="AG10" s="29"/>
-      <c r="AH10" s="29"/>
-      <c r="AI10" s="29"/>
-      <c r="AM10" s="29"/>
-      <c r="AN10" s="29"/>
-      <c r="AO10" s="29"/>
-      <c r="AP10" s="29"/>
-      <c r="AQ10" s="29"/>
-      <c r="AR10" s="29"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="27"/>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="27"/>
+      <c r="AH10" s="27"/>
+      <c r="AI10" s="27"/>
+      <c r="AM10" s="27"/>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="27"/>
+      <c r="AQ10" s="27"/>
+      <c r="AR10" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AQ9:AQ10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AG10"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AI9:AI10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="AD5:AF5"/>
     <mergeCell ref="AG5:AI5"/>
     <mergeCell ref="AM5:AO5"/>
@@ -1411,6 +1390,30 @@
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="U5:W5"/>
     <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AQ9:AQ10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Mise à jour des branchements.
</commit_message>
<xml_diff>
--- a/Branchements.xlsx
+++ b/Branchements.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main Board" sheetId="1" r:id="rId1"/>
+    <sheet name="Carte Processeur" sheetId="1" r:id="rId1"/>
     <sheet name="Relais" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Aller</t>
   </si>
@@ -118,13 +118,38 @@
   </si>
   <si>
     <t>Vers Alim Secours Transfo 12V</t>
+  </si>
+  <si>
+    <t>Alim 12v1</t>
+  </si>
+  <si>
+    <t>Alim 12v2</t>
+  </si>
+  <si>
+    <t>Cable Micro
+USB</t>
+  </si>
+  <si>
+    <t>&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;</t>
+  </si>
+  <si>
+    <t>(non présent)</t>
+  </si>
+  <si>
+    <t>+ 12V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + 12V2 (non present)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +157,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +207,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightUp">
+        <fgColor auto="1"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -303,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -322,42 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -367,6 +398,55 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,6 +454,340 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1123947</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38103</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur en arc 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5410197" y="1304925"/>
+          <a:ext cx="2371728" cy="1476377"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1000127</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161927</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connecteur en arc 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4624390" y="1462089"/>
+          <a:ext cx="3695697" cy="1476373"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDot"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>933451</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connecteur en arc 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4248151" y="2295525"/>
+          <a:ext cx="2238375" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1038226</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connecteur en arc 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4352926" y="2295525"/>
+          <a:ext cx="2238375" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1152526</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Connecteur en arc 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4467226" y="2305050"/>
+          <a:ext cx="2238375" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connecteur en arc 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4143375" y="2295525"/>
+          <a:ext cx="2238375" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -661,27 +1075,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:R11"/>
+  <dimension ref="B2:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="R19" sqref="R18:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="6" width="2.28515625" customWidth="1"/>
-    <col min="7" max="7" width="0.5703125" customWidth="1"/>
-    <col min="8" max="9" width="2.28515625" customWidth="1"/>
-    <col min="10" max="10" width="0.5703125" customWidth="1"/>
-    <col min="11" max="12" width="2.28515625" customWidth="1"/>
-    <col min="13" max="13" width="0.5703125" customWidth="1"/>
-    <col min="14" max="15" width="2.28515625" customWidth="1"/>
-    <col min="16" max="16" width="0.5703125" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="4.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="1"/>
+    <col min="6" max="7" width="2.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="0.5703125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="2.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="0.5703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="2.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="0.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="2.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="0.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="3.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="1"/>
+    <col min="22" max="22" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18">
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="2:22">
+      <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -695,11 +1117,20 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" spans="3:18">
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22">
+      <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -713,14 +1144,18 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="7"/>
-    </row>
-    <row r="4" spans="3:18">
-      <c r="C4" s="16" t="s">
+      <c r="R3" s="6"/>
+      <c r="S3" s="7"/>
+    </row>
+    <row r="4" spans="2:22">
+      <c r="B4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -733,12 +1168,22 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="7"/>
-    </row>
-    <row r="5" spans="3:18">
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="15" customHeight="1">
+      <c r="B5" s="33"/>
+      <c r="C5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -751,12 +1196,14 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="7"/>
-    </row>
-    <row r="6" spans="3:18">
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="2:22">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -769,11 +1216,11 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" spans="3:18">
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="2:22">
+      <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -787,106 +1234,125 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" spans="3:18">
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="2:22">
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="13"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" spans="3:18">
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="22" t="s">
+      <c r="R8" s="6"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="2:22">
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="G9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="9"/>
+      <c r="L9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="M9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="P9" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="R9" s="10"/>
-    </row>
-    <row r="10" spans="3:18" ht="21" customHeight="1">
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="25"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="25"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="25"/>
-    </row>
-    <row r="11" spans="3:18" ht="80.25" customHeight="1">
-      <c r="E11" s="26" t="s">
+      <c r="R9" s="9"/>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="2:22" ht="21" customHeight="1">
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="23"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="23"/>
+    </row>
+    <row r="11" spans="2:22" ht="80.25" customHeight="1">
+      <c r="F11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="24"/>
+      <c r="I11" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="26"/>
-      <c r="K11" s="26" t="s">
+      <c r="J11" s="24"/>
+      <c r="L11" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="N11" s="26" t="s">
+      <c r="M11" s="24"/>
+      <c r="O11" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="O11" s="26"/>
+      <c r="P11" s="24"/>
+    </row>
+    <row r="13" spans="2:22" ht="15.75">
+      <c r="V13" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="10.5" customHeight="1"/>
+    <row r="16" spans="2:22" ht="15.75">
+      <c r="R16" s="36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="22:22" ht="15.75">
+      <c r="V17" s="37" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N11:O11"/>
+  <mergeCells count="14">
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:E6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="L9:L10"/>
-    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="M9:M10"/>
     <mergeCell ref="O9:O10"/>
-    <mergeCell ref="C4:D6"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="P9:P10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -895,7 +1361,7 @@
   <dimension ref="B2:AS10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1052,64 +1518,64 @@
     </row>
     <row r="5" spans="2:45" ht="79.5" customHeight="1">
       <c r="B5" s="5"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="7"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="28" t="s">
+      <c r="M5" s="17"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="18"/>
       <c r="R5" s="7"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="28" t="s">
+      <c r="U5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="28" t="s">
+      <c r="V5" s="17"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="30"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="18"/>
       <c r="AA5" s="7"/>
       <c r="AC5" s="5"/>
-      <c r="AD5" s="28" t="s">
+      <c r="AD5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="28" t="s">
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AH5" s="29"/>
-      <c r="AI5" s="30"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="18"/>
       <c r="AJ5" s="7"/>
       <c r="AL5" s="5"/>
-      <c r="AM5" s="28" t="s">
+      <c r="AM5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AN5" s="29"/>
-      <c r="AO5" s="30"/>
-      <c r="AP5" s="28" t="s">
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AQ5" s="29"/>
-      <c r="AR5" s="30"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="18"/>
       <c r="AS5" s="7"/>
     </row>
     <row r="6" spans="2:45" ht="4.5" customHeight="1">
@@ -1240,140 +1706,164 @@
     </row>
     <row r="9" spans="2:45" s="6" customFormat="1" ht="7.5" customHeight="1">
       <c r="B9" s="8"/>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="19" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="10"/>
       <c r="K9" s="8"/>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="O9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="27" t="s">
+      <c r="P9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="27" t="s">
+      <c r="Q9" s="19" t="s">
         <v>18</v>
       </c>
       <c r="R9" s="10"/>
       <c r="T9" s="8"/>
-      <c r="U9" s="27" t="s">
+      <c r="U9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="V9" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="W9" s="27" t="s">
+      <c r="X9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="X9" s="27" t="s">
+      <c r="Z9" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="Y9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z9" s="27" t="s">
-        <v>24</v>
       </c>
       <c r="AA9" s="10"/>
       <c r="AC9" s="8"/>
-      <c r="AD9" s="27" t="s">
+      <c r="AD9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AE9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF9" s="27" t="s">
+      <c r="AG9" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AG9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH9" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI9" s="27" t="s">
+      <c r="AI9" s="19" t="s">
         <v>26</v>
       </c>
       <c r="AJ9" s="10"/>
       <c r="AL9" s="8"/>
-      <c r="AM9" s="27" t="s">
+      <c r="AM9" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AN9" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO9" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="AP9" s="27" t="s">
+      <c r="AP9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="AQ9" s="27" t="s">
+      <c r="AQ9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="AR9" s="27" t="s">
+      <c r="AR9" s="19" t="s">
         <v>31</v>
       </c>
       <c r="AS9" s="10"/>
     </row>
     <row r="10" spans="2:45" ht="144.75" customHeight="1">
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AM10" s="27"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
-      <c r="AR10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
+      <c r="AI10" s="19"/>
+      <c r="AM10" s="19"/>
+      <c r="AN10" s="19"/>
+      <c r="AO10" s="19"/>
+      <c r="AP10" s="19"/>
+      <c r="AQ10" s="19"/>
+      <c r="AR10" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="AR9:AR10"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="AN9:AN10"/>
+    <mergeCell ref="AO9:AO10"/>
+    <mergeCell ref="AP9:AP10"/>
+    <mergeCell ref="AQ9:AQ10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
     <mergeCell ref="AD5:AF5"/>
     <mergeCell ref="AG5:AI5"/>
     <mergeCell ref="AM5:AO5"/>
@@ -1390,30 +1880,6 @@
     <mergeCell ref="O5:Q5"/>
     <mergeCell ref="U5:W5"/>
     <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="AR9:AR10"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AG9:AG10"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AI9:AI10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="AN9:AN10"/>
-    <mergeCell ref="AO9:AO10"/>
-    <mergeCell ref="AP9:AP10"/>
-    <mergeCell ref="AQ9:AQ10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>